<commit_message>
start annual review prep
</commit_message>
<xml_diff>
--- a/data/students.xlsx
+++ b/data/students.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00315273\Documents\GitHub\jy_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E026110E-90E6-4455-914E-1C3DB6514F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DAD9D6-72FB-45C6-A725-0556B07A9133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="1493" windowWidth="19365" windowHeight="12187" xr2:uid="{E8785A74-FE56-4D65-A4F0-E49533BAE9B0}"/>
+    <workbookView xWindow="33405" yWindow="780" windowWidth="20325" windowHeight="14655" xr2:uid="{E8785A74-FE56-4D65-A4F0-E49533BAE9B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="119">
   <si>
     <t>with</t>
   </si>
@@ -282,9 +282,6 @@
     <t>Investigating the Effectiveness  of Explicit,  Systematic  Mathematics Vocabulary  Instruction  for  Students in  Fourth  Grade</t>
   </si>
   <si>
-    <t>Executivve Functioning in Children With ASD and Co-Occurring Neurodevelopmental Disorders: A Systematic Review and Quantitative Analysis</t>
-  </si>
-  <si>
     <t>Kristen Rolf</t>
   </si>
   <si>
@@ -340,13 +337,67 @@
   </si>
   <si>
     <t>Aug 2019</t>
+  </si>
+  <si>
+    <t>ADHD knowledge and its relationship to stigma and treatment decisions among parents</t>
+  </si>
+  <si>
+    <t>Executive Functioning in Children with ASD and Co-occurring Neurodevelopmental Disorders: A Systematic Review and Quantitative Analysis</t>
+  </si>
+  <si>
+    <t>Dec 2021</t>
+  </si>
+  <si>
+    <t>Olysola Omisakin</t>
+  </si>
+  <si>
+    <t>Sociology</t>
+  </si>
+  <si>
+    <t>BMI trajectories in the AddHealth</t>
+  </si>
+  <si>
+    <t>Mulilevel Modeling with Multiple Imputations</t>
+  </si>
+  <si>
+    <t>Psychology - Brain and Cognition</t>
+  </si>
+  <si>
+    <t>Stephanie (Crank) Avila</t>
+  </si>
+  <si>
+    <t>Language influene on deception and its detection</t>
+  </si>
+  <si>
+    <t>Expected defense: Spring 2023</t>
+  </si>
+  <si>
+    <t>Ben Juarez</t>
+  </si>
+  <si>
+    <t>Psychology - Clinical Counseling</t>
+  </si>
+  <si>
+    <t>Mentor: Dr. Chris Warren</t>
+  </si>
+  <si>
+    <t>Mentor: Dr. Eric Reither</t>
+  </si>
+  <si>
+    <t>Mentor: Dr. Melanie Domenech Rodriguez</t>
+  </si>
+  <si>
+    <t>Proposal defense: April 13, 2022</t>
+  </si>
+  <si>
+    <t>CRIES-8 Validation with Latinx Youth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +433,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -404,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -421,6 +479,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -736,24 +795,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE0E004-468D-403D-8056-2F867B2BC815}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="23.59765625" customWidth="1"/>
-    <col min="6" max="6" width="13.59765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.796875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="14.3984375" customWidth="1"/>
-    <col min="9" max="9" width="37.19921875" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -780,7 +839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -797,26 +856,29 @@
         <v>39</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
       <c r="I2" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I3" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I4" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -833,29 +895,26 @@
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
       <c r="I6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -872,7 +931,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>17</v>
@@ -881,17 +940,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -908,7 +967,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>27</v>
@@ -917,17 +976,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I14" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -944,21 +1003,21 @@
         <v>8</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
@@ -975,7 +1034,7 @@
         <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>32</v>
@@ -984,17 +1043,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I18" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1011,7 +1070,7 @@
         <v>45</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>48</v>
@@ -1020,17 +1079,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I21" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1047,7 +1106,7 @@
         <v>58</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>32</v>
@@ -1056,7 +1115,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>13</v>
       </c>
@@ -1064,12 +1123,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I25" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1083,29 +1142,29 @@
         <v>21</v>
       </c>
       <c r="E26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I27" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1119,10 +1178,10 @@
         <v>21</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>32</v>
@@ -1131,17 +1190,17 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I30" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>11</v>
       </c>
@@ -1158,7 +1217,7 @@
         <v>72</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>32</v>
@@ -1167,17 +1226,17 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I33" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>12</v>
       </c>
@@ -1203,17 +1262,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I36" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>13</v>
       </c>
@@ -1236,20 +1295,20 @@
         <v>65</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I39" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I40" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>14</v>
       </c>
@@ -1257,7 +1316,7 @@
         <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D41" t="s">
         <v>21</v>
@@ -1266,7 +1325,7 @@
         <v>79</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>27</v>
@@ -1275,17 +1334,17 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I42" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I43" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>15</v>
       </c>
@@ -1299,29 +1358,29 @@
         <v>21</v>
       </c>
       <c r="E44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G44" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I44" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="I44" s="9" t="s">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="I45" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>16</v>
       </c>
@@ -1341,18 +1400,18 @@
         <v>53</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I48" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>17</v>
       </c>
@@ -1360,7 +1419,7 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D49" t="s">
         <v>21</v>
@@ -1369,26 +1428,26 @@
         <v>45</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="I50" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I51" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>18</v>
       </c>
@@ -1414,17 +1473,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I53" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I54" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>19</v>
       </c>
@@ -1450,17 +1509,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I56" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I57" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>20</v>
       </c>
@@ -1471,7 +1530,7 @@
         <v>40</v>
       </c>
       <c r="D58" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E58" t="s">
         <v>63</v>
@@ -1483,17 +1542,125 @@
         <v>65</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="I59" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I60" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>21</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>40</v>
+      </c>
+      <c r="D61" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" t="s">
+        <v>104</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G61" t="s">
+        <v>105</v>
+      </c>
+      <c r="I61" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I62" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I63" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>22</v>
+      </c>
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" t="s">
+        <v>109</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I65" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I66" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>23</v>
+      </c>
+      <c r="B67" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" t="s">
+        <v>112</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I68" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I69" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1510,6 +1677,6 @@
     <hyperlink ref="I33" r:id="rId10" xr:uid="{595FBA2E-8E09-458F-A4C3-111A47B02FAD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
apply for Business job
</commit_message>
<xml_diff>
--- a/data/students.xlsx
+++ b/data/students.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00315273\Documents\GitHub\jy_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DAD9D6-72FB-45C6-A725-0556B07A9133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CB6BA9-FA5E-4E37-A076-AC7CDAD78EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33405" yWindow="780" windowWidth="20325" windowHeight="14655" xr2:uid="{E8785A74-FE56-4D65-A4F0-E49533BAE9B0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{E8785A74-FE56-4D65-A4F0-E49533BAE9B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="120">
   <si>
     <t>with</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>CRIES-8 Validation with Latinx Youth</t>
+  </si>
+  <si>
+    <t>May 2022</t>
   </si>
 </sst>
 </file>
@@ -797,20 +800,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AE0E004-468D-403D-8056-2F867B2BC815}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.59765625" customWidth="1"/>
+    <col min="6" max="6" width="13.59765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.86328125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.3984375" customWidth="1"/>
+    <col min="9" max="9" width="37.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -839,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -868,17 +871,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I3" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I4" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2</v>
       </c>
@@ -904,17 +907,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>3</v>
       </c>
@@ -940,17 +943,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>4</v>
       </c>
@@ -976,17 +979,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I14" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1012,12 +1015,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I16" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1043,17 +1046,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I18" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1079,22 +1082,22 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I21" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -1115,7 +1118,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>13</v>
       </c>
@@ -1123,12 +1126,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
       <c r="I25" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1154,17 +1157,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I27" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I28" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1190,17 +1193,17 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I30" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>11</v>
       </c>
@@ -1226,17 +1229,17 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I33" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>12</v>
       </c>
@@ -1262,17 +1265,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I36" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I37" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>13</v>
       </c>
@@ -1298,17 +1301,17 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I39" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I40" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>14</v>
       </c>
@@ -1334,17 +1337,17 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I42" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I43" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>15</v>
       </c>
@@ -1352,7 +1355,7 @@
         <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D44" t="s">
         <v>21</v>
@@ -1361,7 +1364,7 @@
         <v>93</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>90</v>
@@ -1370,17 +1373,17 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I45" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I46" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>16</v>
       </c>
@@ -1406,12 +1409,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I48" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>17</v>
       </c>
@@ -1437,17 +1440,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I50" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I51" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>18</v>
       </c>
@@ -1473,17 +1476,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
       <c r="I53" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
       <c r="I54" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>19</v>
       </c>
@@ -1509,17 +1512,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I56" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I57" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>20</v>
       </c>
@@ -1545,17 +1548,17 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15.4" x14ac:dyDescent="0.45">
       <c r="I59" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I60" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>21</v>
       </c>
@@ -1581,17 +1584,17 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I62" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I63" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>22</v>
       </c>
@@ -1617,17 +1620,17 @@
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I65" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I66" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>23</v>
       </c>
@@ -1653,12 +1656,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I68" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="I69" t="s">
         <v>116</v>
       </c>

</xml_diff>